<commit_message>
Changed name of parameter.
</commit_message>
<xml_diff>
--- a/archiveDecoder/sample/description.xlsx
+++ b/archiveDecoder/sample/description.xlsx
@@ -24,12 +24,6 @@
     <t>nameImg_UV</t>
   </si>
   <si>
-    <t>begin_layer</t>
-  </si>
-  <si>
-    <t>end_layer</t>
-  </si>
-  <si>
     <t>part1_DL.jpg</t>
   </si>
   <si>
@@ -52,6 +46,12 @@
   </si>
   <si>
     <t>part4_UV.jpg</t>
+  </si>
+  <si>
+    <t>begin_part</t>
+  </si>
+  <si>
+    <t>end_part</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,18 +414,18 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C2" s="1">
         <v>0</v>
@@ -436,10 +436,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1">
         <v>1.45</v>
@@ -450,10 +450,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1">
         <v>3.54</v>
@@ -464,10 +464,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1">
         <v>5.85</v>

</xml_diff>

<commit_message>
Changed struct of description and made edits in decoder.
</commit_message>
<xml_diff>
--- a/archiveDecoder/sample/description.xlsx
+++ b/archiveDecoder/sample/description.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>nameImg_DL</t>
   </si>
@@ -52,6 +52,15 @@
   </si>
   <si>
     <t>end_part</t>
+  </si>
+  <si>
+    <t>parts</t>
+  </si>
+  <si>
+    <t>deposit</t>
+  </si>
+  <si>
+    <t>hole</t>
   </si>
 </sst>
 </file>
@@ -75,7 +84,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -83,13 +92,212 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -391,7 +599,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
@@ -399,84 +607,107 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" customWidth="1"/>
-    <col min="2" max="2" width="19.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" customWidth="1"/>
-    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="6"/>
+    </row>
+    <row r="2" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2" s="12">
+        <v>2</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F2" s="9" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C3" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1">
+      <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="D2" s="1">
+      <c r="F3" s="11">
         <v>1.45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C4" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1">
+      <c r="E4" s="2">
         <v>1.45</v>
       </c>
-      <c r="D3" s="1">
+      <c r="F4" s="11">
         <v>3.54</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="C5" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="1">
+      <c r="E5" s="2">
         <v>3.54</v>
       </c>
-      <c r="D4" s="1">
+      <c r="F5" s="11">
         <v>5.85</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C6" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D6" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="1">
+      <c r="E6" s="15">
         <v>5.85</v>
       </c>
-      <c r="D5" s="1">
+      <c r="F6" s="16">
         <v>5.93</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>